<commit_message>
Colelcted new results. Added a "pure" golden reference point.
</commit_message>
<xml_diff>
--- a/TrainingResults.xlsx
+++ b/TrainingResults.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t xml:space="preserve">Test ID</t>
   </si>
@@ -70,7 +70,7 @@
     <t xml:space="preserve">A001</t>
   </si>
   <si>
-    <t xml:space="preserve">23/10</t>
+    <t xml:space="preserve">21 10</t>
   </si>
   <si>
     <t xml:space="preserve">Initial 2-class attempt.</t>
@@ -82,16 +82,13 @@
     <t xml:space="preserve">A002</t>
   </si>
   <si>
-    <t xml:space="preserve">29/10</t>
-  </si>
-  <si>
     <t xml:space="preserve">Improving weights for 2-class setup. Also tweaked some weights.</t>
   </si>
   <si>
     <t xml:space="preserve">A003</t>
   </si>
   <si>
-    <t xml:space="preserve">?</t>
+    <t xml:space="preserve">05 11</t>
   </si>
   <si>
     <t xml:space="preserve">Testing if results of the model hold up a second time.</t>
@@ -100,6 +97,9 @@
     <t xml:space="preserve">A004</t>
   </si>
   <si>
+    <t xml:space="preserve">06 11</t>
+  </si>
+  <si>
     <t xml:space="preserve">Testing if results of the model hold up a second time. Again.</t>
   </si>
   <si>
@@ -113,6 +113,39 @@
   </si>
   <si>
     <t xml:space="preserve">ADModel_Strange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilise an alternative, far simpler model (still on old augs).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using simpler model again, this time with less intense augmentation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing the interpolation-based 3D augmentation on a known working path.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make the interpolation augmentation a little less intense.</t>
   </si>
 </sst>
 </file>
@@ -121,13 +154,14 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="YY/MM/DD"/>
+    <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
   </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -149,6 +183,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -261,27 +296,27 @@
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.26020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="54.2295918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.48469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.98469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.51530612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.7091836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.20408163265306"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.5714285714286"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.4591836734694"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.7091836734694"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.20408163265306"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.5714285714286"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.4591836734694"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.4897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="53.5918367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.4744897959184"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.4744897959184"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -381,10 +416,10 @@
         <v>19</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>20</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7" t="n">
@@ -421,16 +456,16 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>24</v>
-      </c>
       <c r="D4" s="6" t="n">
-        <v>0.929</v>
+        <v>0.81</v>
       </c>
       <c r="E4" s="6" t="n">
         <v>0.562</v>
@@ -466,16 +501,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>23</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>0.835</v>
+        <v>0.88</v>
       </c>
       <c r="E5" s="6" t="n">
         <v>0.523</v>
@@ -516,13 +551,13 @@
         <v>28</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D6" s="6" t="n">
-        <v>0.98</v>
+        <v>0.78</v>
       </c>
       <c r="E6" s="6" t="n">
         <v>0.633</v>
@@ -559,72 +594,192 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
+      <c r="A7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="6" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="E7" s="6" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="F7" s="6" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="G7" s="6" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="H7" s="6" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="I7" s="6" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="J7" s="6" t="n">
+        <v>132</v>
+      </c>
+      <c r="K7" s="6" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="L7" s="6" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="M7" s="6" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="N7" s="6" t="n">
+        <v>38</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="6" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="E8" s="6" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="G8" s="6" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="H8" s="6" t="n">
+        <v>0.94</v>
+      </c>
+      <c r="I8" s="6" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="J8" s="6" t="n">
+        <v>132</v>
+      </c>
+      <c r="K8" s="6" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="L8" s="6" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="M8" s="6" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="N8" s="6" t="n">
+        <v>38</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="6" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="E9" s="6" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="F9" s="6" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="G9" s="6" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="H9" s="6" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="I9" s="6" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="J9" s="6" t="n">
+        <v>132</v>
+      </c>
+      <c r="K9" s="6" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="L9" s="6" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="M9" s="6" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N9" s="6" t="n">
+        <v>38</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
+      <c r="A10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="6" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="E10" s="6" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="F10" s="6" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="G10" s="6" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="H10" s="6" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="I10" s="6" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="J10" s="6" t="n">
+        <v>132</v>
+      </c>
+      <c r="K10" s="6" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="L10" s="6" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="M10" s="6" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="N10" s="6" t="n">
+        <v>38</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6"/>

</xml_diff>